<commit_message>
actualizacion de los dos archivos en la carpeta BD y formato asistecia
</commit_message>
<xml_diff>
--- a/Formato_Asistencia_Woman_Consulting_Group.xlsx
+++ b/Formato_Asistencia_Woman_Consulting_Group.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sandra Jimenez\Documents\ANALISIS_DE_DATOS_KEY_CODE\Trabajo Final\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sandra Jimenez\Documents\ANALISIS_DE_DATOS_KEY_CODE\Proyecto Final\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9029348B-84B4-4AEE-9F0C-61E8E27C60DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{277BE826-94B2-44D8-A6EE-1EF53A75BC03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="25">
   <si>
     <t>Nombre</t>
   </si>
@@ -92,23 +92,19 @@
   </si>
   <si>
     <t>x</t>
+  </si>
+  <si>
+    <t>Excusa laboral</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -121,13 +117,34 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="6"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -157,12 +174,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -471,8 +494,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -481,7 +504,7 @@
     <col min="2" max="2" width="9.7265625" customWidth="1"/>
     <col min="3" max="3" width="9.453125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.26953125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.7265625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.7265625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.7265625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.1796875" bestFit="1" customWidth="1"/>
@@ -493,31 +516,31 @@
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="5" t="s">
         <v>22</v>
       </c>
     </row>
@@ -531,8 +554,12 @@
       <c r="C2" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
+      <c r="D2" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>23</v>
+      </c>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
@@ -549,8 +576,12 @@
       <c r="C3" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
+      <c r="D3" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>23</v>
+      </c>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
@@ -567,8 +598,12 @@
       <c r="C4" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
+      <c r="D4" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>23</v>
+      </c>
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
@@ -585,8 +620,12 @@
       <c r="C5" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
+      <c r="D5" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>24</v>
+      </c>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
@@ -600,9 +639,11 @@
       <c r="B6" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="4"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="4" t="s">
+        <v>23</v>
+      </c>
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
@@ -619,8 +660,12 @@
       <c r="C7" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
+      <c r="D7" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>24</v>
+      </c>
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
@@ -637,8 +682,12 @@
       <c r="C8" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
+      <c r="D8" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>23</v>
+      </c>
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
@@ -655,8 +704,10 @@
       <c r="C9" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
+      <c r="D9" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E9" s="4"/>
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
@@ -673,8 +724,12 @@
       <c r="C10" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
+      <c r="D10" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>23</v>
+      </c>
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
@@ -691,8 +746,12 @@
       <c r="C11" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
+      <c r="D11" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>23</v>
+      </c>
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
@@ -709,8 +768,12 @@
       <c r="C12" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
+      <c r="D12" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>23</v>
+      </c>
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
@@ -727,8 +790,10 @@
       <c r="C13" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
+      <c r="D13" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E13" s="4"/>
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
@@ -745,8 +810,12 @@
       <c r="C14" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
+      <c r="D14" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>23</v>
+      </c>
       <c r="F14" s="3"/>
       <c r="G14" s="3"/>
       <c r="H14" s="3"/>

</xml_diff>